<commit_message>
Changes to most major functions
Needed to make the Anomaly report work again so made some changes. Also changed the outliers code to make it only output if outliers are detected
</commit_message>
<xml_diff>
--- a/Data_Cleansing/OXO-5FI696 Augusta_anomaly_report/xlsx/correlations/OXO-5FI696 Augusta corr.xlsx
+++ b/Data_Cleansing/OXO-5FI696 Augusta_anomaly_report/xlsx/correlations/OXO-5FI696 Augusta corr.xlsx
@@ -1,13 +1,13 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Sheet1" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>

</xml_diff>